<commit_message>
modificaciones historia de usuario 003
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>No</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Jez Humble</t>
+  </si>
+  <si>
+    <t>esteban chato</t>
   </si>
 </sst>
 </file>
@@ -422,8 +425,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -492,8 +495,8 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5">
-        <v>102</v>
+      <c r="D5" t="n">
+        <v>102.0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>